<commit_message>
Added ACMG Tier3 data
</commit_message>
<xml_diff>
--- a/data/Dati Input Strategies.xlsx
+++ b/data/Dati Input Strategies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">#disease</t>
   </si>
@@ -31,13 +31,16 @@
     <t xml:space="preserve">Strategy A1 (MS)</t>
   </si>
   <si>
-    <t xml:space="preserve">Strategy A2 (FS)</t>
+    <t xml:space="preserve">Strategy A (FS)</t>
   </si>
   <si>
     <t xml:space="preserve">Strategy C (ACOG)</t>
   </si>
   <si>
     <t xml:space="preserve">Strategy D (ACMG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategy B (ACOG+ACMG)</t>
   </si>
   <si>
     <t xml:space="preserve">Cystic Fibrosis</t>
@@ -206,19 +209,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="8" style="1" width="9.14"/>
   </cols>
@@ -242,13 +246,16 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
@@ -260,6 +267,9 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -268,7 +278,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
@@ -280,6 +290,9 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -288,7 +301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -301,6 +314,9 @@
       </c>
       <c r="F4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,7 +324,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1</v>
@@ -320,6 +336,9 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -328,7 +347,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0</v>
@@ -340,6 +359,9 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -348,7 +370,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
@@ -360,6 +382,9 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -368,7 +393,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
@@ -380,6 +405,9 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -388,7 +416,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
@@ -400,6 +428,9 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -408,7 +439,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -420,6 +451,9 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -428,7 +462,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
@@ -440,6 +474,9 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -448,7 +485,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -460,6 +497,9 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -468,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -480,6 +520,9 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -488,7 +531,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -500,6 +543,9 @@
         <v>0</v>
       </c>
       <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -508,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -520,6 +566,9 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -528,7 +577,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -540,6 +589,9 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -548,7 +600,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -560,6 +612,9 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -568,7 +623,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -580,6 +635,9 @@
         <v>0</v>
       </c>
       <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -588,7 +646,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -600,6 +658,9 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -608,7 +669,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -620,6 +681,9 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -628,7 +692,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -640,6 +704,9 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -648,7 +715,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
@@ -660,6 +727,9 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>